<commit_message>
Adds ability to add players, adds auto loca
</commit_message>
<xml_diff>
--- a/Assets/Game/Data/Localization.xlsx
+++ b/Assets/Game/Data/Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\_private\kid-game\Assets\Game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AA1AED-195F-4D31-BA50-273096E3BC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094E5E0B-AA69-4F15-9265-55E19A0EC9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>Key</t>
   </si>
@@ -106,6 +106,36 @@
   </si>
   <si>
     <t>Nein</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Quit</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>Anwenden</t>
+  </si>
+  <si>
+    <t>Beenden</t>
+  </si>
+  <si>
+    <t>Abbrechen</t>
+  </si>
+  <si>
+    <t>Select Player</t>
+  </si>
+  <si>
+    <t>SelectPlayer</t>
+  </si>
+  <si>
+    <t>Spieler Ändern</t>
   </si>
 </sst>
 </file>
@@ -441,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,13 +588,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D8" t="str">
         <f>""</f>
@@ -573,13 +603,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D9" t="str">
         <f>""</f>
@@ -588,15 +618,90 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D14" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="str">
         <f>""</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Adds loca, cleans up button prefabs
</commit_message>
<xml_diff>
--- a/Assets/Game/Data/Localization.xlsx
+++ b/Assets/Game/Data/Localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\_private\kid-game\Assets\Game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094E5E0B-AA69-4F15-9265-55E19A0EC9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCD81E1-F331-4A74-A949-AFE4B9EDD607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3456" yWindow="3456" windowWidth="23040" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Key</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Spieler Ändern</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Zurück</t>
+  </si>
+  <si>
+    <t>PlayAgain</t>
+  </si>
+  <si>
+    <t>Play Again</t>
+  </si>
+  <si>
+    <t>Nochmal Spielen</t>
   </si>
 </sst>
 </file>
@@ -471,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,6 +717,36 @@
         <v>32</v>
       </c>
       <c r="D15" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="str">
         <f>""</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Unifies visuals across multiple screens and modals
</commit_message>
<xml_diff>
--- a/Assets/Game/Data/Localization.xlsx
+++ b/Assets/Game/Data/Localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\_private\kid-game\Assets\Game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6637E86F-359D-4A6D-AFF5-94A11FE1EA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045996E4-5BA4-4845-B101-28ABD6E77387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Localization" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
   <si>
     <t>Key</t>
   </si>
@@ -295,6 +295,15 @@
   </si>
   <si>
     <t>Hello, {0}!</t>
+  </si>
+  <si>
+    <t>LevelCompleteTitle</t>
+  </si>
+  <si>
+    <t>Great!</t>
+  </si>
+  <si>
+    <t>Super!</t>
   </si>
 </sst>
 </file>
@@ -630,19 +639,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="4" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="4" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -670,7 +679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -684,7 +693,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -698,7 +707,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -712,7 +721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -726,7 +735,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -741,7 +750,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -756,7 +765,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -770,7 +779,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -784,7 +793,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -799,7 +808,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -813,7 +822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -827,7 +836,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -842,7 +851,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -856,7 +865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -870,7 +879,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -884,7 +893,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -898,7 +907,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -912,7 +921,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -926,7 +935,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -940,7 +949,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -954,7 +963,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -968,7 +977,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -982,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -1064,6 +1073,20 @@
       </c>
       <c r="D30" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1080,22 +1103,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Adds credits, links and some visual adjustments to UI
</commit_message>
<xml_diff>
--- a/Assets/Game/Data/Localization.xlsx
+++ b/Assets/Game/Data/Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\_private\kid-game\Assets\Game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045996E4-5BA4-4845-B101-28ABD6E77387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFF5871-150B-471D-8F71-A7481318AD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
   <si>
     <t>Key</t>
   </si>
@@ -304,6 +304,36 @@
   </si>
   <si>
     <t>Super!</t>
+  </si>
+  <si>
+    <t>Credits</t>
+  </si>
+  <si>
+    <t>Mitwirkende</t>
+  </si>
+  <si>
+    <t>Załoga</t>
+  </si>
+  <si>
+    <t>HowToPlay</t>
+  </si>
+  <si>
+    <t>How to Play</t>
+  </si>
+  <si>
+    <t>Spielanleitung</t>
+  </si>
+  <si>
+    <t>Jak Grać</t>
+  </si>
+  <si>
+    <t>OpenSourceNotice</t>
+  </si>
+  <si>
+    <t>This game is open source. You can find it on &lt;color=#A52A2A&gt;&lt;link source="githuburl"&gt;GitHub  \uf35d&lt;/link&gt;&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>Pestępój</t>
   </si>
 </sst>
 </file>
@@ -639,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,9 +775,8 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="str">
-        <f>""</f>
-        <v/>
+      <c r="D7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -760,9 +789,8 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="str">
-        <f>""</f>
-        <v/>
+      <c r="D8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1087,6 +1115,50 @@
       </c>
       <c r="D31" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <f>""</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wires up level end script
</commit_message>
<xml_diff>
--- a/Assets/Game/Data/Localization.xlsx
+++ b/Assets/Game/Data/Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\_private\kid-game\Assets\Game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE8DB5B-A65D-4787-BE67-FB6B76810795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10E94A6-F3FB-4F14-92D1-21ED93F7B1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
   <si>
     <t>Key</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>Great!</t>
-  </si>
-  <si>
-    <t>Super!</t>
   </si>
   <si>
     <t>Credits</t>
@@ -406,6 +403,12 @@
 Chimney, roof, windows, a new door as well.
 And no more did he fear the consequences of bad winter
 But lived peacefully amongst his people.</t>
+  </si>
+  <si>
+    <t>Großartig!</t>
+  </si>
+  <si>
+    <t>Świetnie!</t>
   </si>
 </sst>
 </file>
@@ -746,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +856,7 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1188,46 +1191,46 @@
         <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
         <v>89</v>
       </c>
-      <c r="B32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>90</v>
-      </c>
-      <c r="D32" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
         <v>92</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>93</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>94</v>
-      </c>
-      <c r="D33" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
         <v>96</v>
-      </c>
-      <c r="B34" t="s">
-        <v>97</v>
       </c>
       <c r="C34" t="str">
         <f>""</f>
@@ -1240,7 +1243,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B35" t="str">
         <f>""</f>
@@ -1257,16 +1260,16 @@
     </row>
     <row r="36" spans="1:4" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds simple help screen
</commit_message>
<xml_diff>
--- a/Assets/Game/Data/Localization.xlsx
+++ b/Assets/Game/Data/Localization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\_private\kid-game\Assets\Game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB5FB5E-E3D0-4B29-BAB1-F5A7BAA707A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2204CE5E-20BC-45EB-AE28-EF2D40AC5F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
   <si>
     <t>Key</t>
   </si>
@@ -421,6 +421,27 @@
   </si>
   <si>
     <t>This game is based on an old Polish children's song, passed down orally. The music is based on the melody I was taught, but you might know a slightly different version of it. The same applies to the lyrics, which you can find below.</t>
+  </si>
+  <si>
+    <t>The gnome runs automatically towards his house. Along the way, you can either jump or roll. There are four levels, each becoming progressively more interesting than the last.
+In Levels 1, 2, and 3, you can jump by tapping anywhere on the screen. If you are using a computer, you can click with the mouse or use the spacebar.
+In Level 4, you must also roll away from the owl! To jump, tap the left half of the screen, and to roll, tap the right half of the screen.
+If you are using a computer, you can click with the mouse or use the spacebar to jump, and the Control key to roll.</t>
+  </si>
+  <si>
+    <t>Der Zwerg läuft automatisch zu seinem Haus. Auf dem Weg kannst du entweder springen oder rollen. Es gibt vier Stufen, wobei jede Stufe interessanter als die vorherige wird.
+In Stufe 1, 2 und 3 kannst du springen, indem du irgendwo auf dem Bildschirm tippst. Wenn du einen Computer verwendest, kannst du mit der Maus klicken oder die Leertaste benutzen.
+In Stufe 4 musst du auch vor der Eule wegrollen! Um zu springen, tippe auf die linke Hälfte des Bildschirms, und um zu rollen, tippe auf die rechte Hälfte des Bildschirms.
+Wenn du einen Computer verwendest, kannst du mit der Maus klicken oder die Leertaste zum Springen und die Strg-Taste zum Rollen verwenden.</t>
+  </si>
+  <si>
+    <t>Krasnolud biegnie automatycznie do swojego domu. W trakcie podróży możesz skakać lub toczyć się. Są cztery poziomy, z których każdy jest coraz ciekawszy od poprzedniego.
+Na poziomach 1, 2 i 3 możesz skakać, dotykając dowolnego miejsca na ekranie. Jeśli używasz komputera, możesz kliknąć myszką lub użyć spacji.
+Na poziomie 4 musisz także toczyć się na ziemi, aby uniknąć sowy! Aby skoczyć, dotknij lewej połowy ekranu, a aby się toczyć, dotknij prawej połowy ekranu.
+Jeśli używasz komputera, możesz kliknąć myszką lub użyć spacji do skakania i klawisza Ctrl do toczenia się.</t>
+  </si>
+  <si>
+    <t>HowToPlayDesc</t>
   </si>
 </sst>
 </file>
@@ -759,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,6 +1299,20 @@
       </c>
       <c r="D36" s="3" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds splashscreen logic and loca
</commit_message>
<xml_diff>
--- a/Assets/Game/Data/Localization.xlsx
+++ b/Assets/Game/Data/Localization.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\_private\kid-game\Assets\Game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2204CE5E-20BC-45EB-AE28-EF2D40AC5F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B616F61-B274-4232-80B1-CEFAF888BC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
   <si>
     <t>Key</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>GameName</t>
-  </si>
-  <si>
-    <t>Kid Game</t>
   </si>
   <si>
     <t>PlayerName</t>
@@ -442,6 +439,42 @@
   </si>
   <si>
     <t>HowToPlayDesc</t>
+  </si>
+  <si>
+    <t>Gnome and Owl</t>
+  </si>
+  <si>
+    <t>Gnom und Eule</t>
+  </si>
+  <si>
+    <t>Krasnoludek i Sowa</t>
+  </si>
+  <si>
+    <t>Gnome</t>
+  </si>
+  <si>
+    <t>And</t>
+  </si>
+  <si>
+    <t>Owl</t>
+  </si>
+  <si>
+    <t>Gnom</t>
+  </si>
+  <si>
+    <t>und</t>
+  </si>
+  <si>
+    <t>Eule</t>
+  </si>
+  <si>
+    <t>Krasnoludek</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Sowa</t>
   </si>
 </sst>
 </file>
@@ -780,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,139 +843,139 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="str">
         <f>""</f>
@@ -954,262 +987,262 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>83</v>
@@ -1217,102 +1250,144 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" t="s">
         <v>95</v>
       </c>
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" t="str">
+      <c r="C37" t="str">
         <f>""</f>
         <v/>
       </c>
-      <c r="D34" t="str">
+      <c r="D37" t="str">
         <f>""</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="40" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C35" t="s">
-        <v>107</v>
-      </c>
-      <c r="D35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="345.6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="216" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1341,12 +1416,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unifies settings menu to be in line with other screens
</commit_message>
<xml_diff>
--- a/Assets/Game/Data/Localization.xlsx
+++ b/Assets/Game/Data/Localization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\_private\kid-game\Assets\Game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B616F61-B274-4232-80B1-CEFAF888BC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAFB7AC-9BE9-4938-B8AD-D0F70D99497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -324,9 +324,6 @@
     <t>OpenSourceNotice</t>
   </si>
   <si>
-    <t>This game is open source. You can find it on &lt;color=#A52A2A&gt;&lt;link source="githuburl"&gt;GitHub  \uf35d&lt;/link&gt;&lt;/color&gt;</t>
-  </si>
-  <si>
     <t>Pestępój</t>
   </si>
   <si>
@@ -475,6 +472,9 @@
   </si>
   <si>
     <t>Sowa</t>
+  </si>
+  <si>
+    <t>This game is open source. You can find it on &lt;color=#A52A2A&gt;&lt;link source="githuburl"&gt;GitHub: https://github.com/SMaleck/kid-game&lt;/link&gt;&lt;/color&gt;</t>
   </si>
 </sst>
 </file>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,7 +922,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -987,55 +987,55 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
         <v>112</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>113</v>
-      </c>
-      <c r="D12" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1063,7 +1063,7 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1298,10 +1298,10 @@
         <v>86</v>
       </c>
       <c r="C34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" t="s">
         <v>102</v>
-      </c>
-      <c r="D34" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1337,7 +1337,7 @@
         <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C37" t="str">
         <f>""</f>
@@ -1350,44 +1350,44 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="216" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>